<commit_message>
updated last author list with non-MD scientists
</commit_message>
<xml_diff>
--- a/data/table-last-authors.xlsx
+++ b/data/table-last-authors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giandomenicobisaccia/VS/CMR-publications-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0762473-049F-5D4C-8840-88D011891C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE47AC11-9E6F-D344-B2F2-62DB90849B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1762,13 +1762,13 @@
     <t>Lahey Hospital Medical Center</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Azienda Ospedale Università Padova</t>
   </si>
   <si>
     <t>JOHN P GREENWOOD</t>
+  </si>
+  <si>
+    <t>Non-MD scientist</t>
   </si>
 </sst>
 </file>
@@ -2161,7 +2161,7 @@
   <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2297,7 +2297,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -2374,7 +2374,7 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2517,7 +2517,7 @@
         <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2898,7 +2898,7 @@
         <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -3084,7 +3084,7 @@
         <v>153</v>
       </c>
       <c r="E61" t="s">
-        <v>580</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3752,7 +3752,7 @@
         <v>257</v>
       </c>
       <c r="E104" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -3909,7 +3909,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B115" t="s">
         <v>34</v>
@@ -4055,7 +4055,7 @@
         <v>286</v>
       </c>
       <c r="E125" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -4510,7 +4510,7 @@
         <v>359</v>
       </c>
       <c r="E153" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -4527,7 +4527,7 @@
         <v>97</v>
       </c>
       <c r="E154" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
         <v>23</v>
       </c>
       <c r="E182" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -5271,7 +5271,7 @@
         <v>23</v>
       </c>
       <c r="E202" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -5305,7 +5305,7 @@
         <v>97</v>
       </c>
       <c r="E204" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -5415,7 +5415,7 @@
         <v>23</v>
       </c>
       <c r="E211" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -5618,7 +5618,7 @@
         <v>97</v>
       </c>
       <c r="E224" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -5880,7 +5880,7 @@
         <v>63</v>
       </c>
       <c r="E241" t="s">
-        <v>580</v>
+        <v>28</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>